<commit_message>
Feat: Add Mob Vision
1. 몬스터에 시야 범위가 추가되었으며, 눈 모양 UI 를 통해 이를 확인할 수 있습니다
2. 플레이어를 감지하지 않은 몬스터는 아무런 행동도 하지 않습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\노민\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B764D8ED-72D6-4C69-BDD1-C709520BB562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172F96A3-E319-4CF3-A298-79CFC176FB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6705" yWindow="1455" windowWidth="29625" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Tile_Empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,14 @@
   </si>
   <si>
     <t>Bishop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -476,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0B6F6-72BE-4042-9DBD-113B2542E50A}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BJ4" sqref="BJ4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BC24" sqref="BC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -740,10 +748,10 @@
         <v>0</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -812,10 +820,10 @@
         <v>8</v>
       </c>
       <c r="BI3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="BJ3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -878,10 +886,10 @@
       <c r="BC4" s="3"/>
       <c r="BD4" s="3"/>
       <c r="BI4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BJ4" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -943,6 +951,12 @@
       <c r="BB5" s="3"/>
       <c r="BC5" s="3"/>
       <c r="BD5" s="3"/>
+      <c r="BI5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1873,7 +1887,9 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
+      <c r="AA21" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
@@ -1938,7 +1954,9 @@
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
-      <c r="AF22" s="4"/>
+      <c r="AF22" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
@@ -2051,7 +2069,9 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="Y24" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
@@ -2118,7 +2138,9 @@
       <c r="AC25" s="4"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
+      <c r="AF25" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="AG25" s="4"/>
       <c r="AH25" s="4"/>
       <c r="AI25" s="3"/>
@@ -2169,7 +2191,9 @@
       <c r="T26" s="3"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
+      <c r="W26" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4"/>
@@ -2234,7 +2258,9 @@
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
-      <c r="AB27" s="4"/>
+      <c r="AB27" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="AC27" s="4"/>
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
@@ -2290,7 +2316,9 @@
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
+      <c r="X28" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
       <c r="AA28" s="4"/>
@@ -2415,7 +2443,9 @@
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4"/>
-      <c r="AC30" s="4"/>
+      <c r="AC30" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="AD30" s="4"/>
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
@@ -2472,7 +2502,9 @@
       <c r="W31" s="3"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="Z31" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
       <c r="AC31" s="4"/>
@@ -2536,9 +2568,13 @@
       <c r="AA32" s="4"/>
       <c r="AB32" s="4"/>
       <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
+      <c r="AD32" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
+      <c r="AF32" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="AG32" s="4"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
@@ -2654,7 +2690,9 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
       <c r="AA34" s="4"/>
-      <c r="AB34" s="4"/>
+      <c r="AB34" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="AC34" s="4"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>

</xml_diff>

<commit_message>
Feat: Add Tile Property
1. 이제 타일 속성에 추가 데미지가 들어갑니다.
    1. 현재 타일 상성은 숲 > 물 > 땅 > 숲 이며, 상성 우위는 데미지가 두 배 적용됩니다.
    2. 스킬은 상성이 적용되지 않습니다.
    3. 몬스터의 공격도 상성이 적용됩니다.
2. UI 가 업데이트 되었습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\노민\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172F96A3-E319-4CF3-A298-79CFC176FB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A97763C-E391-4AEF-A723-4A6156239900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="1455" windowWidth="29625" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Tile_Empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,30 @@
     <t>User</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Tile_Forest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tile_Water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tile_Ground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FF6ED749</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FF3FCDFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FF744A0C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +173,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFDE7FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF744A0C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6ED749"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FCDFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +236,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -202,6 +253,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3FCDFF"/>
+      <color rgb="FF6ED749"/>
+      <color rgb="FF744A0C"/>
       <color rgb="FFFDE7FB"/>
       <color rgb="FFFEF4FD"/>
       <color rgb="FFB17ED8"/>
@@ -484,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0B6F6-72BE-4042-9DBD-113B2542E50A}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BC24" sqref="BC24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -885,6 +939,12 @@
       <c r="BB4" s="3"/>
       <c r="BC4" s="3"/>
       <c r="BD4" s="3"/>
+      <c r="BF4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="BI4" s="2" t="s">
         <v>10</v>
       </c>
@@ -951,6 +1011,12 @@
       <c r="BB5" s="3"/>
       <c r="BC5" s="3"/>
       <c r="BD5" s="3"/>
+      <c r="BF5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="BI5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1017,6 +1083,12 @@
       <c r="BB6" s="3"/>
       <c r="BC6" s="3"/>
       <c r="BD6" s="3"/>
+      <c r="BF6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1885,14 +1957,14 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
+      <c r="Y21" s="7"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
@@ -1946,12 +2018,12 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="7"/>
       <c r="AB22" s="4"/>
-      <c r="AC22" s="4"/>
+      <c r="AC22" s="6"/>
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4" t="s">
@@ -2007,17 +2079,17 @@
       <c r="T23" s="3"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
       <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="6"/>
       <c r="AD23" s="4"/>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="4"/>
-      <c r="AG23" s="4"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="7"/>
       <c r="AH23" s="4"/>
       <c r="AI23" s="4"/>
       <c r="AJ23" s="4"/>
@@ -2067,19 +2139,19 @@
       <c r="T24" s="3"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="7"/>
       <c r="Y24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
       <c r="AD24" s="4"/>
-      <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
-      <c r="AG24" s="4"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="5"/>
       <c r="AH24" s="4"/>
       <c r="AI24" s="4"/>
       <c r="AJ24" s="4"/>
@@ -2128,20 +2200,20 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="6"/>
       <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="5"/>
       <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
+      <c r="AC25" s="5"/>
       <c r="AD25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4" t="s">
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AG25" s="4"/>
+      <c r="AG25" s="7"/>
       <c r="AH25" s="4"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="3"/>
@@ -2190,20 +2262,20 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
+      <c r="V26" s="7"/>
       <c r="W26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="5"/>
       <c r="AD26" s="4"/>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
-      <c r="AG26" s="4"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="5"/>
       <c r="AH26" s="4"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
@@ -2252,20 +2324,20 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="4"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="5"/>
       <c r="AH27" s="4"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
@@ -2319,14 +2391,14 @@
       <c r="X28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Y28" s="4"/>
+      <c r="Y28" s="6"/>
       <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
+      <c r="AA28" s="7"/>
       <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
+      <c r="AC28" s="5"/>
       <c r="AD28" s="4"/>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
+      <c r="AE28" s="7"/>
+      <c r="AF28" s="7"/>
       <c r="AG28" s="4"/>
       <c r="AH28" s="4"/>
       <c r="AI28" s="3"/>
@@ -2376,16 +2448,16 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="5"/>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
+      <c r="Y29" s="7"/>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
@@ -2437,17 +2509,17 @@
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="7"/>
       <c r="Z30" s="4"/>
-      <c r="AA30" s="4"/>
-      <c r="AB30" s="4"/>
-      <c r="AC30" s="4" t="s">
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AD30" s="4"/>
-      <c r="AE30" s="4"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
       <c r="AH30" s="3"/>
@@ -2500,16 +2572,16 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
-      <c r="X31" s="4"/>
+      <c r="X31" s="7"/>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="AA31" s="4"/>
-      <c r="AB31" s="4"/>
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="4"/>
-      <c r="AE31" s="4"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6"/>
+      <c r="AE31" s="6"/>
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
       <c r="AH31" s="3"/>
@@ -2564,10 +2636,10 @@
       <c r="W32" s="3"/>
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="Z32" s="5"/>
       <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
       <c r="AD32" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Docs: Balance Mob Stats
1. 몬스터의 행동력을 조절하였습니다.
    1. 난이도가 상향되었습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\노민\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A97763C-E391-4AEF-A723-4A6156239900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9054D9-7D5D-445C-97B6-F90B52925790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0B6F6-72BE-4042-9DBD-113B2542E50A}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR26" sqref="AR26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF28" sqref="AF28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1414,18 +1414,18 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-      <c r="AG12" s="4"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
@@ -1474,18 +1474,18 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="4"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
@@ -1536,18 +1536,18 @@
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
-      <c r="AG14" s="4"/>
-      <c r="AH14" s="4"/>
-      <c r="AI14" s="4"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
@@ -1596,18 +1596,18 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="4"/>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="4"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
@@ -1655,17 +1655,17 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
-      <c r="AG16" s="4"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
@@ -1715,11 +1715,11 @@
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
       <c r="AD17" s="4"/>
@@ -1958,11 +1958,11 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="7"/>
-      <c r="Z21" s="4"/>
+      <c r="Z21" s="7"/>
       <c r="AA21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AB21" s="4"/>
+      <c r="AB21" s="6"/>
       <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="4"/>
@@ -1974,7 +1974,7 @@
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
+      <c r="AN21" s="3"/>
       <c r="AO21" s="3"/>
       <c r="AP21" s="3"/>
       <c r="AQ21" s="3"/>
@@ -2022,10 +2022,10 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="7"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="6"/>
       <c r="AF22" s="4" t="s">
         <v>6</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="AK22" s="4"/>
       <c r="AL22" s="4"/>
       <c r="AM22" s="4"/>
-      <c r="AN22" s="4"/>
+      <c r="AN22" s="3"/>
       <c r="AO22" s="3"/>
       <c r="AP22" s="3"/>
       <c r="AQ22" s="3"/>
@@ -2085,8 +2085,8 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="7"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="4"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="6"/>
       <c r="AE23" s="5"/>
       <c r="AF23" s="5"/>
       <c r="AG23" s="7"/>
@@ -2095,8 +2095,8 @@
       <c r="AJ23" s="4"/>
       <c r="AK23" s="4"/>
       <c r="AL23" s="4"/>
-      <c r="AM23" s="4"/>
-      <c r="AN23" s="4"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
       <c r="AO23" s="3"/>
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
@@ -2141,7 +2141,7 @@
       <c r="V24" s="4"/>
       <c r="W24" s="6"/>
       <c r="X24" s="7"/>
-      <c r="Y24" s="4" t="s">
+      <c r="Y24" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Z24" s="4"/>
@@ -2156,9 +2156,9 @@
       <c r="AI24" s="4"/>
       <c r="AJ24" s="4"/>
       <c r="AK24" s="3"/>
-      <c r="AL24" s="4"/>
-      <c r="AM24" s="4"/>
-      <c r="AN24" s="4"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
       <c r="AO24" s="3"/>
       <c r="AP24" s="3"/>
       <c r="AQ24" s="3"/>
@@ -2203,12 +2203,12 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="6"/>
-      <c r="Y25" s="4"/>
+      <c r="Y25" s="6"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="5"/>
-      <c r="AB25" s="4"/>
+      <c r="AB25" s="7"/>
       <c r="AC25" s="5"/>
-      <c r="AD25" s="4"/>
+      <c r="AD25" s="5"/>
       <c r="AE25" s="6"/>
       <c r="AF25" s="5" t="s">
         <v>12</v>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="X26" s="5"/>
       <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
+      <c r="Z26" s="5"/>
       <c r="AA26" s="6"/>
       <c r="AB26" s="7"/>
       <c r="AC26" s="5"/>
@@ -2324,16 +2324,16 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="4"/>
-      <c r="V27" s="5"/>
+      <c r="V27" s="7"/>
       <c r="W27" s="5"/>
-      <c r="X27" s="4"/>
+      <c r="X27" s="7"/>
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
-      <c r="AA27" s="4"/>
+      <c r="AA27" s="5"/>
       <c r="AB27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AC27" s="4"/>
+      <c r="AC27" s="7"/>
       <c r="AD27" s="5"/>
       <c r="AE27" s="6"/>
       <c r="AF27" s="7"/>
@@ -2387,16 +2387,16 @@
       <c r="T28" s="3"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4" t="s">
+      <c r="W28" s="7"/>
+      <c r="X28" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Y28" s="6"/>
       <c r="Z28" s="4"/>
       <c r="AA28" s="7"/>
-      <c r="AB28" s="4"/>
+      <c r="AB28" s="7"/>
       <c r="AC28" s="5"/>
-      <c r="AD28" s="4"/>
+      <c r="AD28" s="5"/>
       <c r="AE28" s="7"/>
       <c r="AF28" s="7"/>
       <c r="AG28" s="4"/>
@@ -2452,10 +2452,10 @@
       <c r="W29" s="5"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="7"/>
-      <c r="Z29" s="4"/>
+      <c r="Z29" s="7"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
+      <c r="AC29" s="7"/>
       <c r="AD29" s="6"/>
       <c r="AE29" s="6"/>
       <c r="AF29" s="4"/>
@@ -2512,15 +2512,15 @@
       <c r="W30" s="7"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="7"/>
-      <c r="Z30" s="4"/>
+      <c r="Z30" s="5"/>
       <c r="AA30" s="5"/>
       <c r="AB30" s="6"/>
       <c r="AC30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AD30" s="6"/>
+      <c r="AD30" s="7"/>
       <c r="AE30" s="6"/>
-      <c r="AF30" s="4"/>
+      <c r="AF30" s="5"/>
       <c r="AG30" s="4"/>
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
@@ -2573,16 +2573,16 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="4"/>
+      <c r="Y31" s="6"/>
       <c r="Z31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AA31" s="4"/>
+      <c r="AA31" s="6"/>
       <c r="AB31" s="7"/>
       <c r="AC31" s="6"/>
       <c r="AD31" s="6"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="4"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="5"/>
       <c r="AG31" s="4"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
@@ -2637,13 +2637,13 @@
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
       <c r="Z32" s="5"/>
-      <c r="AA32" s="4"/>
+      <c r="AA32" s="6"/>
       <c r="AB32" s="7"/>
       <c r="AC32" s="7"/>
-      <c r="AD32" s="4" t="s">
+      <c r="AD32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AE32" s="4"/>
+      <c r="AE32" s="5"/>
       <c r="AF32" s="4" t="s">
         <v>10</v>
       </c>
@@ -2701,12 +2701,12 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="6"/>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="6"/>
       <c r="AG33" s="4"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
@@ -2761,11 +2761,11 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
-      <c r="AA34" s="4"/>
-      <c r="AB34" s="4" t="s">
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AC34" s="4"/>
+      <c r="AC34" s="6"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
@@ -2824,8 +2824,8 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
       <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
-      <c r="AC35" s="4"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>

</xml_diff>

<commit_message>
Feat: Add Package "SuperTiled2Unity"
1. Tiled >> Unity 컨버팅 패키지를 설치하였습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\노민\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC2125F-EC3D-4FB8-B4FC-570E0C261FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DB3B9-B962-44A6-97C2-FFC4862E7579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1160" yWindow="1600" windowWidth="29060" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map0" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="27">
   <si>
     <t>Tile_Empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +129,10 @@
   </si>
   <si>
     <t>I_S</t>
+  </si>
+  <si>
+    <t>Tile Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -556,25 +560,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0B6F6-72BE-4042-9DBD-113B2542E50A}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AM36" sqref="AM36"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BG10" sqref="BG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.625" style="2"/>
-    <col min="57" max="57" width="10.875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="5.58203125" style="2"/>
+    <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
     <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
     <col min="59" max="59" width="34.5" style="2" customWidth="1"/>
-    <col min="60" max="60" width="10.875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="25.125" style="2" customWidth="1"/>
-    <col min="62" max="62" width="28.375" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="5.625" style="2"/>
+    <col min="60" max="60" width="10.83203125" style="2" customWidth="1"/>
+    <col min="61" max="61" width="25.08203125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="2" customWidth="1"/>
+    <col min="63" max="16384" width="5.58203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -754,7 +758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -826,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -898,7 +902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -970,7 +974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1174,7 +1178,7 @@
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
     </row>
-    <row r="8" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1233,8 +1237,11 @@
       <c r="BB8" s="3"/>
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
-    </row>
-    <row r="9" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BG8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1294,7 +1301,7 @@
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
     </row>
-    <row r="10" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1354,7 +1361,7 @@
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
     </row>
-    <row r="11" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1414,7 +1421,7 @@
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
     </row>
-    <row r="12" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1474,7 +1481,7 @@
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
     </row>
-    <row r="13" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1534,7 +1541,7 @@
       <c r="BC13" s="3"/>
       <c r="BD13" s="3"/>
     </row>
-    <row r="14" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1594,7 +1601,7 @@
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
     </row>
-    <row r="15" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1654,7 +1661,7 @@
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
     </row>
-    <row r="16" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1714,7 +1721,7 @@
       <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
     </row>
-    <row r="17" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1774,7 +1781,7 @@
       <c r="BC17" s="3"/>
       <c r="BD17" s="3"/>
     </row>
-    <row r="18" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1834,7 +1841,7 @@
       <c r="BC18" s="3"/>
       <c r="BD18" s="3"/>
     </row>
-    <row r="19" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1894,7 +1901,7 @@
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
     </row>
-    <row r="20" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1954,7 +1961,7 @@
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
     </row>
-    <row r="21" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2014,7 +2021,7 @@
       <c r="BC21" s="3"/>
       <c r="BD21" s="3"/>
     </row>
-    <row r="22" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2074,7 +2081,7 @@
       <c r="BC22" s="3"/>
       <c r="BD22" s="3"/>
     </row>
-    <row r="23" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2134,7 +2141,7 @@
       <c r="BC23" s="3"/>
       <c r="BD23" s="3"/>
     </row>
-    <row r="24" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2194,7 +2201,7 @@
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
     </row>
-    <row r="25" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2254,7 +2261,7 @@
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
     </row>
-    <row r="26" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2314,7 +2321,7 @@
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
     </row>
-    <row r="27" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2374,7 +2381,7 @@
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
     </row>
-    <row r="28" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2434,7 +2441,7 @@
       <c r="BC28" s="3"/>
       <c r="BD28" s="3"/>
     </row>
-    <row r="29" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2494,7 +2501,7 @@
       <c r="BC29" s="3"/>
       <c r="BD29" s="3"/>
     </row>
-    <row r="30" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2554,7 +2561,7 @@
       <c r="BC30" s="3"/>
       <c r="BD30" s="3"/>
     </row>
-    <row r="31" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2614,7 +2621,7 @@
       <c r="BC31" s="3"/>
       <c r="BD31" s="3"/>
     </row>
-    <row r="32" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2676,7 +2683,7 @@
       <c r="BC32" s="3"/>
       <c r="BD32" s="3"/>
     </row>
-    <row r="33" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2736,7 +2743,7 @@
       <c r="BC33" s="3"/>
       <c r="BD33" s="3"/>
     </row>
-    <row r="34" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2796,7 +2803,7 @@
       <c r="BC34" s="3"/>
       <c r="BD34" s="3"/>
     </row>
-    <row r="35" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2858,7 +2865,7 @@
       <c r="BC35" s="3"/>
       <c r="BD35" s="3"/>
     </row>
-    <row r="36" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2918,7 +2925,7 @@
       <c r="BC36" s="3"/>
       <c r="BD36" s="3"/>
     </row>
-    <row r="37" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2978,7 +2985,7 @@
       <c r="BC37" s="3"/>
       <c r="BD37" s="3"/>
     </row>
-    <row r="38" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3053,21 +3060,21 @@
       <selection activeCell="AL41" sqref="AL41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.625" style="2"/>
-    <col min="57" max="57" width="10.875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="5.58203125" style="2"/>
+    <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
     <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
     <col min="59" max="59" width="34.5" style="2" customWidth="1"/>
-    <col min="60" max="60" width="10.875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="25.125" style="2" customWidth="1"/>
-    <col min="62" max="62" width="28.375" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="5.625" style="2"/>
+    <col min="60" max="60" width="10.83203125" style="2" customWidth="1"/>
+    <col min="61" max="61" width="25.08203125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="2" customWidth="1"/>
+    <col min="63" max="16384" width="5.58203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -3247,7 +3254,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3319,7 +3326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3391,7 +3398,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3463,7 +3470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3535,7 +3542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3607,7 +3614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3667,7 +3674,7 @@
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
     </row>
-    <row r="8" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3727,7 +3734,7 @@
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
     </row>
-    <row r="9" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3787,7 +3794,7 @@
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
     </row>
-    <row r="10" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3847,7 +3854,7 @@
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
     </row>
-    <row r="11" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3907,7 +3914,7 @@
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
     </row>
-    <row r="12" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3967,7 +3974,7 @@
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
     </row>
-    <row r="13" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4027,7 +4034,7 @@
       <c r="BC13" s="3"/>
       <c r="BD13" s="3"/>
     </row>
-    <row r="14" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4087,7 +4094,7 @@
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
     </row>
-    <row r="15" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4147,7 +4154,7 @@
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
     </row>
-    <row r="16" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4207,7 +4214,7 @@
       <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
     </row>
-    <row r="17" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4267,7 +4274,7 @@
       <c r="BC17" s="3"/>
       <c r="BD17" s="3"/>
     </row>
-    <row r="18" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4327,7 +4334,7 @@
       <c r="BC18" s="3"/>
       <c r="BD18" s="3"/>
     </row>
-    <row r="19" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4387,7 +4394,7 @@
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
     </row>
-    <row r="20" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4447,7 +4454,7 @@
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
     </row>
-    <row r="21" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4509,7 +4516,7 @@
       <c r="BC21" s="3"/>
       <c r="BD21" s="3"/>
     </row>
-    <row r="22" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4571,7 +4578,7 @@
       <c r="BC22" s="3"/>
       <c r="BD22" s="3"/>
     </row>
-    <row r="23" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4631,7 +4638,7 @@
       <c r="BC23" s="3"/>
       <c r="BD23" s="3"/>
     </row>
-    <row r="24" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4693,7 +4700,7 @@
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
     </row>
-    <row r="25" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4755,7 +4762,7 @@
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
     </row>
-    <row r="26" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4817,7 +4824,7 @@
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
     </row>
-    <row r="27" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4879,7 +4886,7 @@
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
     </row>
-    <row r="28" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4941,7 +4948,7 @@
       <c r="BC28" s="3"/>
       <c r="BD28" s="3"/>
     </row>
-    <row r="29" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5001,7 +5008,7 @@
       <c r="BC29" s="3"/>
       <c r="BD29" s="3"/>
     </row>
-    <row r="30" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5063,7 +5070,7 @@
       <c r="BC30" s="3"/>
       <c r="BD30" s="3"/>
     </row>
-    <row r="31" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5125,7 +5132,7 @@
       <c r="BC31" s="3"/>
       <c r="BD31" s="3"/>
     </row>
-    <row r="32" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5189,7 +5196,7 @@
       <c r="BC32" s="3"/>
       <c r="BD32" s="3"/>
     </row>
-    <row r="33" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5249,7 +5256,7 @@
       <c r="BC33" s="3"/>
       <c r="BD33" s="3"/>
     </row>
-    <row r="34" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5313,7 +5320,7 @@
       <c r="BC34" s="3"/>
       <c r="BD34" s="3"/>
     </row>
-    <row r="35" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5373,7 +5380,7 @@
       <c r="BC35" s="3"/>
       <c r="BD35" s="3"/>
     </row>
-    <row r="36" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5433,7 +5440,7 @@
       <c r="BC36" s="3"/>
       <c r="BD36" s="3"/>
     </row>
-    <row r="37" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5493,7 +5500,7 @@
       <c r="BC37" s="3"/>
       <c r="BD37" s="3"/>
     </row>
-    <row r="38" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5568,21 +5575,21 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="30" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.625" style="2"/>
-    <col min="57" max="57" width="10.875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="5.58203125" style="2"/>
+    <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
     <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
     <col min="59" max="59" width="34.5" style="2" customWidth="1"/>
-    <col min="60" max="60" width="10.875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="25.125" style="2" customWidth="1"/>
-    <col min="62" max="62" width="28.375" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="5.625" style="2"/>
+    <col min="60" max="60" width="10.83203125" style="2" customWidth="1"/>
+    <col min="61" max="61" width="25.08203125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="2" customWidth="1"/>
+    <col min="63" max="16384" width="5.58203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -5762,7 +5769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5834,7 +5841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5906,7 +5913,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5978,7 +5985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -6050,7 +6057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6122,7 +6129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -6182,7 +6189,7 @@
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
     </row>
-    <row r="8" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -6242,7 +6249,7 @@
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
     </row>
-    <row r="9" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -6302,7 +6309,7 @@
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
     </row>
-    <row r="10" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -6362,7 +6369,7 @@
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
     </row>
-    <row r="11" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -6422,7 +6429,7 @@
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
     </row>
-    <row r="12" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -6482,7 +6489,7 @@
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
     </row>
-    <row r="13" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -6542,7 +6549,7 @@
       <c r="BC13" s="3"/>
       <c r="BD13" s="3"/>
     </row>
-    <row r="14" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -6602,7 +6609,7 @@
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
     </row>
-    <row r="15" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -6662,7 +6669,7 @@
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
     </row>
-    <row r="16" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -6722,7 +6729,7 @@
       <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
     </row>
-    <row r="17" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -6782,7 +6789,7 @@
       <c r="BC17" s="3"/>
       <c r="BD17" s="3"/>
     </row>
-    <row r="18" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -6842,7 +6849,7 @@
       <c r="BC18" s="3"/>
       <c r="BD18" s="3"/>
     </row>
-    <row r="19" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -6902,7 +6909,7 @@
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
     </row>
-    <row r="20" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -6962,7 +6969,7 @@
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
     </row>
-    <row r="21" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -7024,7 +7031,7 @@
       <c r="BC21" s="3"/>
       <c r="BD21" s="3"/>
     </row>
-    <row r="22" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -7086,7 +7093,7 @@
       <c r="BC22" s="3"/>
       <c r="BD22" s="3"/>
     </row>
-    <row r="23" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -7146,7 +7153,7 @@
       <c r="BC23" s="3"/>
       <c r="BD23" s="3"/>
     </row>
-    <row r="24" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -7208,7 +7215,7 @@
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
     </row>
-    <row r="25" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -7270,7 +7277,7 @@
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
     </row>
-    <row r="26" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -7332,7 +7339,7 @@
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
     </row>
-    <row r="27" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -7394,7 +7401,7 @@
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
     </row>
-    <row r="28" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -7456,7 +7463,7 @@
       <c r="BC28" s="3"/>
       <c r="BD28" s="3"/>
     </row>
-    <row r="29" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -7516,7 +7523,7 @@
       <c r="BC29" s="3"/>
       <c r="BD29" s="3"/>
     </row>
-    <row r="30" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -7578,7 +7585,7 @@
       <c r="BC30" s="3"/>
       <c r="BD30" s="3"/>
     </row>
-    <row r="31" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -7640,7 +7647,7 @@
       <c r="BC31" s="3"/>
       <c r="BD31" s="3"/>
     </row>
-    <row r="32" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -7704,7 +7711,7 @@
       <c r="BC32" s="3"/>
       <c r="BD32" s="3"/>
     </row>
-    <row r="33" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -7764,7 +7771,7 @@
       <c r="BC33" s="3"/>
       <c r="BD33" s="3"/>
     </row>
-    <row r="34" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -7828,7 +7835,7 @@
       <c r="BC34" s="3"/>
       <c r="BD34" s="3"/>
     </row>
-    <row r="35" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -7888,7 +7895,7 @@
       <c r="BC35" s="3"/>
       <c r="BD35" s="3"/>
     </row>
-    <row r="36" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -7948,7 +7955,7 @@
       <c r="BC36" s="3"/>
       <c r="BD36" s="3"/>
     </row>
-    <row r="37" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -8008,7 +8015,7 @@
       <c r="BC37" s="3"/>
       <c r="BD37" s="3"/>
     </row>
-    <row r="38" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -8082,21 +8089,21 @@
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="30" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.625" style="2"/>
-    <col min="57" max="57" width="10.875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="5.58203125" style="2"/>
+    <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
     <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
     <col min="59" max="59" width="34.5" style="2" customWidth="1"/>
-    <col min="60" max="60" width="10.875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="25.125" style="2" customWidth="1"/>
-    <col min="62" max="62" width="28.375" style="2" customWidth="1"/>
-    <col min="63" max="16384" width="5.625" style="2"/>
+    <col min="60" max="60" width="10.83203125" style="2" customWidth="1"/>
+    <col min="61" max="61" width="25.08203125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="2" customWidth="1"/>
+    <col min="63" max="16384" width="5.58203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>1</v>
@@ -8276,7 +8283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8348,7 +8355,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8420,7 +8427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8492,7 +8499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8564,7 +8571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -8636,7 +8643,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -8696,7 +8703,7 @@
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
     </row>
-    <row r="8" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -8756,7 +8763,7 @@
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
     </row>
-    <row r="9" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -8816,7 +8823,7 @@
       <c r="BC9" s="3"/>
       <c r="BD9" s="3"/>
     </row>
-    <row r="10" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -8876,7 +8883,7 @@
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
     </row>
-    <row r="11" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -8936,7 +8943,7 @@
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
     </row>
-    <row r="12" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -8996,7 +9003,7 @@
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
     </row>
-    <row r="13" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9056,7 +9063,7 @@
       <c r="BC13" s="3"/>
       <c r="BD13" s="3"/>
     </row>
-    <row r="14" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9116,7 +9123,7 @@
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
     </row>
-    <row r="15" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9176,7 +9183,7 @@
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
     </row>
-    <row r="16" spans="1:62" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9236,7 +9243,7 @@
       <c r="BC16" s="3"/>
       <c r="BD16" s="3"/>
     </row>
-    <row r="17" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9296,7 +9303,7 @@
       <c r="BC17" s="3"/>
       <c r="BD17" s="3"/>
     </row>
-    <row r="18" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9356,7 +9363,7 @@
       <c r="BC18" s="3"/>
       <c r="BD18" s="3"/>
     </row>
-    <row r="19" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9416,7 +9423,7 @@
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
     </row>
-    <row r="20" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9476,7 +9483,7 @@
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
     </row>
-    <row r="21" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9538,7 +9545,7 @@
       <c r="BC21" s="3"/>
       <c r="BD21" s="3"/>
     </row>
-    <row r="22" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9600,7 +9607,7 @@
       <c r="BC22" s="3"/>
       <c r="BD22" s="3"/>
     </row>
-    <row r="23" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9660,7 +9667,7 @@
       <c r="BC23" s="3"/>
       <c r="BD23" s="3"/>
     </row>
-    <row r="24" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9722,7 +9729,7 @@
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
     </row>
-    <row r="25" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9784,7 +9791,7 @@
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
     </row>
-    <row r="26" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9846,7 +9853,7 @@
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
     </row>
-    <row r="27" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9908,7 +9915,7 @@
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
     </row>
-    <row r="28" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9970,7 +9977,7 @@
       <c r="BC28" s="3"/>
       <c r="BD28" s="3"/>
     </row>
-    <row r="29" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -10030,7 +10037,7 @@
       <c r="BC29" s="3"/>
       <c r="BD29" s="3"/>
     </row>
-    <row r="30" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -10092,7 +10099,7 @@
       <c r="BC30" s="3"/>
       <c r="BD30" s="3"/>
     </row>
-    <row r="31" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -10154,7 +10161,7 @@
       <c r="BC31" s="3"/>
       <c r="BD31" s="3"/>
     </row>
-    <row r="32" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -10218,7 +10225,7 @@
       <c r="BC32" s="3"/>
       <c r="BD32" s="3"/>
     </row>
-    <row r="33" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -10278,7 +10285,7 @@
       <c r="BC33" s="3"/>
       <c r="BD33" s="3"/>
     </row>
-    <row r="34" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -10342,7 +10349,7 @@
       <c r="BC34" s="3"/>
       <c r="BD34" s="3"/>
     </row>
-    <row r="35" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -10402,7 +10409,7 @@
       <c r="BC35" s="3"/>
       <c r="BD35" s="3"/>
     </row>
-    <row r="36" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -10462,7 +10469,7 @@
       <c r="BC36" s="3"/>
       <c r="BD36" s="3"/>
     </row>
-    <row r="37" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -10522,7 +10529,7 @@
       <c r="BC37" s="3"/>
       <c r="BD37" s="3"/>
     </row>
-    <row r="38" spans="1:56" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Feat: Add Tiled Map
1. 레이어 정렬이 완료되었습니다.
2. Tiled 와 동기화가 완료되었습니다.
3. Map0 이 추가되었습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DB3B9-B962-44A6-97C2-FFC4862E7579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EA457-6DB3-42A8-B269-FD58CCE6D3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1160" yWindow="1600" windowWidth="29060" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map0" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
   <si>
     <t>Tile_Empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB0B6F6-72BE-4042-9DBD-113B2542E50A}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BG10" sqref="BG10"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AP29" sqref="AP29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1338,7 +1338,7 @@
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
+      <c r="AI10" s="4"/>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
@@ -1388,17 +1388,17 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
       <c r="AL11" s="3"/>
@@ -1443,25 +1443,25 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="T12" s="4"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
       <c r="AM12" s="3"/>
       <c r="AN12" s="3"/>
       <c r="AO12" s="3"/>
@@ -1500,28 +1500,28 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
-      <c r="AJ13" s="3"/>
-      <c r="AK13" s="3"/>
-      <c r="AL13" s="3"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
       <c r="AM13" s="3"/>
       <c r="AN13" s="3"/>
       <c r="AO13" s="3"/>
@@ -1559,26 +1559,26 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="3"/>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
@@ -1621,24 +1621,26 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG15" s="4"/>
+      <c r="AH15" s="4"/>
+      <c r="AI15" s="4"/>
       <c r="AJ15" s="3"/>
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
@@ -1682,24 +1684,24 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
-      <c r="AJ16" s="3"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+      <c r="AG16" s="4"/>
+      <c r="AH16" s="4"/>
+      <c r="AI16" s="4"/>
+      <c r="AJ16" s="4"/>
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
       <c r="AM16" s="3"/>
@@ -1741,24 +1743,24 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
@@ -1794,15 +1796,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -1812,10 +1814,10 @@
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
@@ -1852,16 +1854,16 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
@@ -1872,9 +1874,9 @@
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
@@ -1914,27 +1916,27 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
@@ -1974,28 +1976,28 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
@@ -2034,28 +2036,32 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
@@ -2094,32 +2100,32 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="4"/>
+      <c r="AJ23" s="4"/>
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="3"/>
@@ -2127,7 +2133,7 @@
       <c r="AO23" s="3"/>
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
-      <c r="AR23" s="3"/>
+      <c r="AR23" s="4"/>
       <c r="AS23" s="3"/>
       <c r="AT23" s="3"/>
       <c r="AU23" s="3"/>
@@ -2153,30 +2159,30 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="3"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
       <c r="AJ24" s="3"/>
@@ -2186,8 +2192,8 @@
       <c r="AN24" s="3"/>
       <c r="AO24" s="3"/>
       <c r="AP24" s="3"/>
-      <c r="AQ24" s="3"/>
-      <c r="AR24" s="3"/>
+      <c r="AQ24" s="4"/>
+      <c r="AR24" s="4"/>
       <c r="AS24" s="3"/>
       <c r="AT24" s="3"/>
       <c r="AU24" s="3"/>
@@ -2214,29 +2220,29 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+      <c r="AG25" s="4"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
       <c r="AJ25" s="3"/>
@@ -2244,10 +2250,10 @@
       <c r="AL25" s="3"/>
       <c r="AM25" s="3"/>
       <c r="AN25" s="3"/>
-      <c r="AO25" s="3"/>
-      <c r="AP25" s="3"/>
-      <c r="AQ25" s="3"/>
-      <c r="AR25" s="3"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="4"/>
+      <c r="AQ25" s="4"/>
+      <c r="AR25" s="4"/>
       <c r="AS25" s="3"/>
       <c r="AT25" s="3"/>
       <c r="AU25" s="3"/>
@@ -2274,40 +2280,42 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4"/>
+      <c r="AH26" s="4"/>
+      <c r="AI26" s="4"/>
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
       <c r="AL26" s="3"/>
-      <c r="AM26" s="3"/>
-      <c r="AN26" s="3"/>
-      <c r="AO26" s="3"/>
-      <c r="AP26" s="3"/>
-      <c r="AQ26" s="3"/>
-      <c r="AR26" s="3"/>
+      <c r="AM26" s="4"/>
+      <c r="AN26" s="4"/>
+      <c r="AO26" s="4"/>
+      <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
+      <c r="AR26" s="4"/>
       <c r="AS26" s="3"/>
       <c r="AT26" s="3"/>
       <c r="AU26" s="3"/>
@@ -2333,38 +2341,38 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-      <c r="Z27" s="3"/>
-      <c r="AA27" s="3"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="3"/>
-      <c r="AI27" s="3"/>
-      <c r="AJ27" s="3"/>
-      <c r="AK27" s="3"/>
-      <c r="AL27" s="3"/>
-      <c r="AM27" s="3"/>
-      <c r="AN27" s="3"/>
-      <c r="AO27" s="3"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+      <c r="AG27" s="4"/>
+      <c r="AH27" s="4"/>
+      <c r="AI27" s="4"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
       <c r="AP27" s="3"/>
       <c r="AQ27" s="3"/>
       <c r="AR27" s="3"/>
@@ -2392,28 +2400,28 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
@@ -2452,27 +2460,27 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
@@ -2528,9 +2536,9 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
@@ -2587,10 +2595,12 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA31" s="4"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
@@ -2646,13 +2656,11 @@
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
@@ -2708,10 +2716,10 @@
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
       <c r="AA33" s="4"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
@@ -2768,10 +2776,10 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
       <c r="AA34" s="4"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
@@ -2830,8 +2838,8 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="3"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
       <c r="AA35" s="4" t="s">
         <v>8</v>
       </c>
@@ -2894,7 +2902,7 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
-      <c r="AA36" s="3"/>
+      <c r="AA36" s="4"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
@@ -2954,7 +2962,7 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
+      <c r="AA37" s="4"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>

</xml_diff>

<commit_message>
Style: Update UI Inventory
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EA457-6DB3-42A8-B269-FD58CCE6D3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AF65B-DA38-478B-83D5-28329D26AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="27">
   <si>
     <t>Tile_Empty</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -561,7 +561,7 @@
   <dimension ref="A1:BJ38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AP29" sqref="AP29"/>
+      <selection activeCell="AO35" sqref="AO35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2779,7 +2779,9 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+      <c r="Z34" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA34" s="4"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>

</xml_diff>

<commit_message>
Style: Polish Mob Attack Animation
1. 이제 몬스터가 제자리에서 공격합니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B52310-4604-4930-9408-539724D74F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C80C2-85DD-454B-94A5-3DF1DE067A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="2340" windowWidth="26720" windowHeight="14940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="2340" windowWidth="26720" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map0" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="26">
   <si>
     <t>Tile_Water</t>
   </si>
@@ -100,6 +100,10 @@
   </si>
   <si>
     <t>Enemy_Knight</t>
+  </si>
+  <si>
+    <t>E_P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -711,8 +715,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="N7" zoomScale="20" zoomScaleNormal="20" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="AK30" sqref="AK30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2747,7 +2751,7 @@
       <c r="X31" s="3"/>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AA31" s="4"/>
       <c r="AB31" s="3"/>
@@ -13263,7 +13267,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="30" zoomScaleNormal="30" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="R1" zoomScale="30" zoomScaleNormal="30" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Style: Polish Mob Animation
1. 모든 몬스터의 애니메이션 작업이 완료되었습니다.
2. 로딩 화면에 애니메이션을 추가하였습니다.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C80C2-85DD-454B-94A5-3DF1DE067A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E02CC6-8561-496F-9020-E08BD40E7879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="2340" windowWidth="26720" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="27">
   <si>
     <t>Tile_Water</t>
   </si>
@@ -102,7 +102,11 @@
     <t>Enemy_Knight</t>
   </si>
   <si>
-    <t>E_P</t>
+    <t>E_N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_B</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -715,8 +719,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2929,7 +2933,9 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="4"/>
+      <c r="W34" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>

</xml_diff>

<commit_message>
Feat: Add Tutorial 3
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80E47C9-5FD9-4277-A02A-D18B97284551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62557CA-0A1A-4926-BD04-C8FDBF192D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map0" sheetId="8" r:id="rId1"/>
     <sheet name="Map1" sheetId="9" r:id="rId2"/>
-    <sheet name="Map1 (2)" sheetId="10" r:id="rId3"/>
-    <sheet name="Map00" sheetId="1" r:id="rId4"/>
+    <sheet name="Map2" sheetId="10" r:id="rId3"/>
+    <sheet name="Map3" sheetId="1" r:id="rId4"/>
     <sheet name="Map11" sheetId="2" r:id="rId5"/>
     <sheet name="Map22" sheetId="3" r:id="rId6"/>
     <sheet name="Map33" sheetId="4" r:id="rId7"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="32">
   <si>
     <t>Tile_Water</t>
   </si>
@@ -109,15 +109,27 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>E_B</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>U</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>E_P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_S</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_B</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2161,7 +2173,7 @@
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
@@ -2583,7 +2595,7 @@
       <c r="Z28" s="3"/>
       <c r="AA28" s="3"/>
       <c r="AB28" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
@@ -3065,7 +3077,7 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
       <c r="AB36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
@@ -5441,7 +5453,7 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
       <c r="AB34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
@@ -5723,7 +5735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A4D35B-FB9C-4020-A4CB-73CCFA17EEAE}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P22" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="P22" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="AG31" sqref="AG31"/>
     </sheetView>
   </sheetViews>
@@ -7453,10 +7465,10 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
@@ -7699,7 +7711,7 @@
       <c r="Z30" s="4"/>
       <c r="AA30" s="4"/>
       <c r="AB30" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC30" s="4"/>
       <c r="AD30" s="4" t="s">
@@ -7763,10 +7775,10 @@
       <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
       <c r="AB31" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD31" s="4"/>
       <c r="AE31" s="4"/>
@@ -7947,7 +7959,7 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
       <c r="AB34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
@@ -8230,8 +8242,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9721,10 +9733,14 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
+      <c r="AB22" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
+      <c r="AE22" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AF22" s="4"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
@@ -9834,11 +9850,15 @@
       <c r="R24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S24" s="4"/>
+      <c r="S24" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
+      <c r="W24" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
@@ -9893,8 +9913,12 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
+      <c r="R25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
@@ -9902,7 +9926,9 @@
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
+      <c r="AA25" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="4"/>
@@ -10079,7 +10105,9 @@
       <c r="Q28" s="3"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
+      <c r="T28" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="U28" s="4"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
@@ -10146,8 +10174,12 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
+      <c r="AA29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB29" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AC29" s="4"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
@@ -10265,9 +10297,7 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="4"/>
-      <c r="Z31" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="Z31" s="4"/>
       <c r="AA31" s="4"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
@@ -10387,7 +10417,9 @@
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
+      <c r="Z33" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="AA33" s="4"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
@@ -10444,9 +10476,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="W34" s="4"/>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>

</xml_diff>

<commit_message>
Style: Polish Mouse Cursor
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Map.xlsx
+++ b/Assets/StreamingAssets/Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onlym\Desktop\프로그래밍\유니티 리포지토리\2024-Unity.Capstone\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA1E9B2-8B20-4209-B16F-4759C487AB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3783004-ED47-4ED4-BC44-D8E3FAFB0CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="2920" windowWidth="24700" windowHeight="12670" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map0" sheetId="8" r:id="rId1"/>
@@ -19,18 +19,19 @@
     <sheet name="Map3" sheetId="10" r:id="rId4"/>
     <sheet name="Map4" sheetId="1" r:id="rId5"/>
     <sheet name="Map5" sheetId="11" r:id="rId6"/>
-    <sheet name="Map11" sheetId="2" r:id="rId7"/>
-    <sheet name="Map22" sheetId="3" r:id="rId8"/>
-    <sheet name="Map33" sheetId="4" r:id="rId9"/>
-    <sheet name="Map44" sheetId="5" r:id="rId10"/>
-    <sheet name="Map55" sheetId="6" r:id="rId11"/>
+    <sheet name="Map6" sheetId="14" r:id="rId7"/>
+    <sheet name="Map7" sheetId="3" r:id="rId8"/>
+    <sheet name="Map8" sheetId="4" r:id="rId9"/>
+    <sheet name="Map9" sheetId="5" r:id="rId10"/>
+    <sheet name="Map10" sheetId="6" r:id="rId11"/>
+    <sheet name="Map99" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="46">
   <si>
     <t>Tile_Water</t>
   </si>
@@ -156,6 +157,38 @@
   </si>
   <si>
     <t>E_B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_S</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_P</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item_Turn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_C</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3301,7 +3334,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="30" zoomScaleNormal="30" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="AY60" sqref="AY60"/>
     </sheetView>
   </sheetViews>
@@ -5817,7 +5850,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="30" zoomScaleNormal="30" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="L6" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
@@ -8317,6 +8350,2524 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:BJ38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="20" zoomScaleNormal="20" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="20" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" style="2" customWidth="1"/>
+    <col min="22" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5.58203125" style="2"/>
+    <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
+    <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
+    <col min="59" max="59" width="34.5" style="2" customWidth="1"/>
+    <col min="60" max="60" width="10.83203125" style="2" customWidth="1"/>
+    <col min="61" max="61" width="25.08203125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="28.33203125" style="2" customWidth="1"/>
+    <col min="63" max="16384" width="5.58203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BF2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3"/>
+      <c r="AY3" s="3"/>
+      <c r="AZ3" s="3"/>
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BF3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AX4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
+      <c r="BB4" s="3"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BF4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3"/>
+      <c r="AY5" s="3"/>
+      <c r="AZ5" s="3"/>
+      <c r="BA5" s="3"/>
+      <c r="BB5" s="3"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BF5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BJ5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BF6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="BI6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="AY7" s="3"/>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+    </row>
+    <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
+      <c r="AT8" s="3"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="3"/>
+      <c r="AX8" s="3"/>
+      <c r="AY8" s="3"/>
+      <c r="AZ8" s="3"/>
+      <c r="BA8" s="3"/>
+      <c r="BB8" s="3"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+    </row>
+    <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="3"/>
+      <c r="AU9" s="3"/>
+      <c r="AV9" s="3"/>
+      <c r="AW9" s="3"/>
+      <c r="AX9" s="3"/>
+      <c r="AY9" s="3"/>
+      <c r="AZ9" s="3"/>
+      <c r="BA9" s="3"/>
+      <c r="BB9" s="3"/>
+      <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
+    </row>
+    <row r="10" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
+      <c r="AS10" s="3"/>
+      <c r="AT10" s="3"/>
+      <c r="AU10" s="3"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="3"/>
+      <c r="AX10" s="3"/>
+      <c r="AY10" s="3"/>
+      <c r="AZ10" s="3"/>
+      <c r="BA10" s="3"/>
+      <c r="BB10" s="3"/>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+    </row>
+    <row r="11" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="3"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
+      <c r="AS11" s="3"/>
+      <c r="AT11" s="3"/>
+      <c r="AU11" s="3"/>
+      <c r="AV11" s="3"/>
+      <c r="AW11" s="3"/>
+      <c r="AX11" s="3"/>
+      <c r="AY11" s="3"/>
+      <c r="AZ11" s="3"/>
+      <c r="BA11" s="3"/>
+      <c r="BB11" s="3"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+    </row>
+    <row r="12" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="3"/>
+      <c r="AU12" s="3"/>
+      <c r="AV12" s="3"/>
+      <c r="AW12" s="3"/>
+      <c r="AX12" s="3"/>
+      <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
+      <c r="BA12" s="3"/>
+      <c r="BB12" s="3"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+    </row>
+    <row r="13" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AT13" s="3"/>
+      <c r="AU13" s="3"/>
+      <c r="AV13" s="3"/>
+      <c r="AW13" s="3"/>
+      <c r="AX13" s="3"/>
+      <c r="AY13" s="3"/>
+      <c r="AZ13" s="3"/>
+      <c r="BA13" s="3"/>
+      <c r="BB13" s="3"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+    </row>
+    <row r="14" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+      <c r="AU14" s="3"/>
+      <c r="AV14" s="3"/>
+      <c r="AW14" s="3"/>
+      <c r="AX14" s="3"/>
+      <c r="AY14" s="3"/>
+      <c r="AZ14" s="3"/>
+      <c r="BA14" s="3"/>
+      <c r="BB14" s="3"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+    </row>
+    <row r="15" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="3"/>
+      <c r="AO15" s="3"/>
+      <c r="AP15" s="3"/>
+      <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="3"/>
+      <c r="AU15" s="3"/>
+      <c r="AV15" s="3"/>
+      <c r="AW15" s="3"/>
+      <c r="AX15" s="3"/>
+      <c r="AY15" s="3"/>
+      <c r="AZ15" s="3"/>
+      <c r="BA15" s="3"/>
+      <c r="BB15" s="3"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+    </row>
+    <row r="16" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="4"/>
+      <c r="AM16" s="4"/>
+      <c r="AN16" s="4"/>
+      <c r="AO16" s="3"/>
+      <c r="AP16" s="3"/>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="3"/>
+      <c r="AT16" s="3"/>
+      <c r="AU16" s="3"/>
+      <c r="AV16" s="3"/>
+      <c r="AW16" s="3"/>
+      <c r="AX16" s="3"/>
+      <c r="AY16" s="3"/>
+      <c r="AZ16" s="3"/>
+      <c r="BA16" s="3"/>
+      <c r="BB16" s="3"/>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+    </row>
+    <row r="17" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="4"/>
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3"/>
+      <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
+      <c r="AS17" s="3"/>
+      <c r="AT17" s="3"/>
+      <c r="AU17" s="3"/>
+      <c r="AV17" s="3"/>
+      <c r="AW17" s="3"/>
+      <c r="AX17" s="3"/>
+      <c r="AY17" s="3"/>
+      <c r="AZ17" s="3"/>
+      <c r="BA17" s="3"/>
+      <c r="BB17" s="3"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+    </row>
+    <row r="18" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="3"/>
+      <c r="AP18" s="3"/>
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
+      <c r="AS18" s="3"/>
+      <c r="AT18" s="3"/>
+      <c r="AU18" s="3"/>
+      <c r="AV18" s="3"/>
+      <c r="AW18" s="3"/>
+      <c r="AX18" s="3"/>
+      <c r="AY18" s="3"/>
+      <c r="AZ18" s="3"/>
+      <c r="BA18" s="3"/>
+      <c r="BB18" s="3"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+    </row>
+    <row r="19" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="3"/>
+      <c r="AP19" s="3"/>
+      <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
+      <c r="AS19" s="3"/>
+      <c r="AT19" s="3"/>
+      <c r="AU19" s="3"/>
+      <c r="AV19" s="3"/>
+      <c r="AW19" s="3"/>
+      <c r="AX19" s="3"/>
+      <c r="AY19" s="3"/>
+      <c r="AZ19" s="3"/>
+      <c r="BA19" s="3"/>
+      <c r="BB19" s="3"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+    </row>
+    <row r="20" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="3"/>
+      <c r="AP20" s="3"/>
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
+      <c r="AS20" s="3"/>
+      <c r="AT20" s="3"/>
+      <c r="AU20" s="3"/>
+      <c r="AV20" s="3"/>
+      <c r="AW20" s="3"/>
+      <c r="AX20" s="3"/>
+      <c r="AY20" s="3"/>
+      <c r="AZ20" s="3"/>
+      <c r="BA20" s="3"/>
+      <c r="BB20" s="3"/>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+    </row>
+    <row r="21" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="4"/>
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="3"/>
+      <c r="AP21" s="3"/>
+      <c r="AQ21" s="3"/>
+      <c r="AR21" s="3"/>
+      <c r="AS21" s="3"/>
+      <c r="AT21" s="3"/>
+      <c r="AU21" s="3"/>
+      <c r="AV21" s="3"/>
+      <c r="AW21" s="3"/>
+      <c r="AX21" s="3"/>
+      <c r="AY21" s="3"/>
+      <c r="AZ21" s="3"/>
+      <c r="BA21" s="3"/>
+      <c r="BB21" s="3"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+    </row>
+    <row r="22" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="3"/>
+      <c r="AO22" s="3"/>
+      <c r="AP22" s="3"/>
+      <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+      <c r="AU22" s="3"/>
+      <c r="AV22" s="3"/>
+      <c r="AW22" s="3"/>
+      <c r="AX22" s="3"/>
+      <c r="AY22" s="3"/>
+      <c r="AZ22" s="3"/>
+      <c r="BA22" s="3"/>
+      <c r="BB22" s="3"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="3"/>
+    </row>
+    <row r="23" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+      <c r="AG23" s="4"/>
+      <c r="AH23" s="4"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="3"/>
+      <c r="AY23" s="3"/>
+      <c r="AZ23" s="3"/>
+      <c r="BA23" s="3"/>
+      <c r="BB23" s="3"/>
+      <c r="BC23" s="3"/>
+      <c r="BD23" s="3"/>
+    </row>
+    <row r="24" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+      <c r="AG24" s="4"/>
+      <c r="AH24" s="4"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="3"/>
+      <c r="AX24" s="3"/>
+      <c r="AY24" s="3"/>
+      <c r="AZ24" s="3"/>
+      <c r="BA24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+    </row>
+    <row r="25" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+      <c r="AW25" s="3"/>
+      <c r="AX25" s="3"/>
+      <c r="AY25" s="3"/>
+      <c r="AZ25" s="3"/>
+      <c r="BA25" s="3"/>
+      <c r="BB25" s="3"/>
+      <c r="BC25" s="3"/>
+      <c r="BD25" s="3"/>
+    </row>
+    <row r="26" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+      <c r="AW26" s="3"/>
+      <c r="AX26" s="3"/>
+      <c r="AY26" s="3"/>
+      <c r="AZ26" s="3"/>
+      <c r="BA26" s="3"/>
+      <c r="BB26" s="3"/>
+      <c r="BC26" s="3"/>
+      <c r="BD26" s="3"/>
+    </row>
+    <row r="27" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="3"/>
+      <c r="AO27" s="3"/>
+      <c r="AP27" s="3"/>
+      <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
+      <c r="AS27" s="3"/>
+      <c r="AT27" s="3"/>
+      <c r="AU27" s="3"/>
+      <c r="AV27" s="3"/>
+      <c r="AW27" s="3"/>
+      <c r="AX27" s="3"/>
+      <c r="AY27" s="3"/>
+      <c r="AZ27" s="3"/>
+      <c r="BA27" s="3"/>
+      <c r="BB27" s="3"/>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+    </row>
+    <row r="28" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="3"/>
+      <c r="AO28" s="3"/>
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="3"/>
+      <c r="AU28" s="3"/>
+      <c r="AV28" s="3"/>
+      <c r="AW28" s="3"/>
+      <c r="AX28" s="3"/>
+      <c r="AY28" s="3"/>
+      <c r="AZ28" s="3"/>
+      <c r="BA28" s="3"/>
+      <c r="BB28" s="3"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="3"/>
+    </row>
+    <row r="29" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="4"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="3"/>
+      <c r="AP29" s="3"/>
+      <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
+      <c r="AS29" s="3"/>
+      <c r="AT29" s="3"/>
+      <c r="AU29" s="3"/>
+      <c r="AV29" s="3"/>
+      <c r="AW29" s="3"/>
+      <c r="AX29" s="3"/>
+      <c r="AY29" s="3"/>
+      <c r="AZ29" s="3"/>
+      <c r="BA29" s="3"/>
+      <c r="BB29" s="3"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="3"/>
+    </row>
+    <row r="30" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="4"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="4"/>
+      <c r="AN30" s="3"/>
+      <c r="AO30" s="3"/>
+      <c r="AP30" s="3"/>
+      <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
+      <c r="AS30" s="3"/>
+      <c r="AT30" s="3"/>
+      <c r="AU30" s="3"/>
+      <c r="AV30" s="3"/>
+      <c r="AW30" s="3"/>
+      <c r="AX30" s="3"/>
+      <c r="AY30" s="3"/>
+      <c r="AZ30" s="3"/>
+      <c r="BA30" s="3"/>
+      <c r="BB30" s="3"/>
+      <c r="BC30" s="3"/>
+      <c r="BD30" s="3"/>
+    </row>
+    <row r="31" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="4"/>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+      <c r="AG31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH31" s="4"/>
+      <c r="AI31" s="4"/>
+      <c r="AJ31" s="4"/>
+      <c r="AK31" s="4"/>
+      <c r="AL31" s="4"/>
+      <c r="AM31" s="4"/>
+      <c r="AN31" s="3"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="3"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+      <c r="BD31" s="3"/>
+    </row>
+    <row r="32" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="4"/>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="4"/>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+      <c r="AG32" s="4"/>
+      <c r="AH32" s="4"/>
+      <c r="AI32" s="4"/>
+      <c r="AJ32" s="4"/>
+      <c r="AK32" s="4"/>
+      <c r="AL32" s="4"/>
+      <c r="AM32" s="4"/>
+      <c r="AN32" s="3"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="3"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+      <c r="BD32" s="3"/>
+    </row>
+    <row r="33" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="4"/>
+      <c r="AJ33" s="4"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="4"/>
+      <c r="AM33" s="4"/>
+      <c r="AN33" s="3"/>
+      <c r="AO33" s="3"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
+      <c r="AV33" s="3"/>
+      <c r="AW33" s="3"/>
+      <c r="AX33" s="3"/>
+      <c r="AY33" s="3"/>
+      <c r="AZ33" s="3"/>
+      <c r="BA33" s="3"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+      <c r="BD33" s="3"/>
+    </row>
+    <row r="34" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="4"/>
+      <c r="AM34" s="4"/>
+      <c r="AN34" s="3"/>
+      <c r="AO34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+      <c r="AU34" s="3"/>
+      <c r="AV34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="AX34" s="3"/>
+      <c r="AY34" s="3"/>
+      <c r="AZ34" s="3"/>
+      <c r="BA34" s="3"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+      <c r="BD34" s="3"/>
+    </row>
+    <row r="35" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="4"/>
+      <c r="AC35" s="4"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="4"/>
+      <c r="AI35" s="4"/>
+      <c r="AJ35" s="4"/>
+      <c r="AK35" s="4"/>
+      <c r="AL35" s="4"/>
+      <c r="AM35" s="4"/>
+      <c r="AN35" s="3"/>
+      <c r="AO35" s="3"/>
+      <c r="AP35" s="3"/>
+      <c r="AQ35" s="3"/>
+      <c r="AR35" s="3"/>
+      <c r="AS35" s="3"/>
+      <c r="AT35" s="3"/>
+      <c r="AU35" s="3"/>
+      <c r="AV35" s="3"/>
+      <c r="AW35" s="3"/>
+      <c r="AX35" s="3"/>
+      <c r="AY35" s="3"/>
+      <c r="AZ35" s="3"/>
+      <c r="BA35" s="3"/>
+      <c r="BB35" s="3"/>
+      <c r="BC35" s="3"/>
+      <c r="BD35" s="3"/>
+    </row>
+    <row r="36" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3"/>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="3"/>
+      <c r="AO36" s="3"/>
+      <c r="AP36" s="3"/>
+      <c r="AQ36" s="3"/>
+      <c r="AR36" s="3"/>
+      <c r="AS36" s="3"/>
+      <c r="AT36" s="3"/>
+      <c r="AU36" s="3"/>
+      <c r="AV36" s="3"/>
+      <c r="AW36" s="3"/>
+      <c r="AX36" s="3"/>
+      <c r="AY36" s="3"/>
+      <c r="AZ36" s="3"/>
+      <c r="BA36" s="3"/>
+      <c r="BB36" s="3"/>
+      <c r="BC36" s="3"/>
+      <c r="BD36" s="3"/>
+    </row>
+    <row r="37" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+      <c r="AG37" s="3"/>
+      <c r="AH37" s="3"/>
+      <c r="AI37" s="3"/>
+      <c r="AJ37" s="3"/>
+      <c r="AK37" s="3"/>
+      <c r="AL37" s="3"/>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+      <c r="AU37" s="3"/>
+      <c r="AV37" s="3"/>
+      <c r="AW37" s="3"/>
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="3"/>
+      <c r="AZ37" s="3"/>
+      <c r="BA37" s="3"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+      <c r="BD37" s="3"/>
+    </row>
+    <row r="38" spans="1:56" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3"/>
+      <c r="AL38" s="3"/>
+      <c r="AM38" s="3"/>
+      <c r="AN38" s="3"/>
+      <c r="AO38" s="3"/>
+      <c r="AP38" s="3"/>
+      <c r="AQ38" s="3"/>
+      <c r="AR38" s="3"/>
+      <c r="AS38" s="3"/>
+      <c r="AT38" s="3"/>
+      <c r="AU38" s="3"/>
+      <c r="AV38" s="3"/>
+      <c r="AW38" s="3"/>
+      <c r="AX38" s="3"/>
+      <c r="AY38" s="3"/>
+      <c r="AZ38" s="3"/>
+      <c r="BA38" s="3"/>
+      <c r="BB38" s="3"/>
+      <c r="BC38" s="3"/>
+      <c r="BD38" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -18416,7 +20967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76C3C83-1721-4B70-92DF-84051E7EE42B}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N24" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="N24" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
@@ -20919,20 +23470,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D95F09-A38F-4180-A713-459B521A8719}">
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="20" zoomScaleNormal="20" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="AO33" sqref="AO33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="9" width="5.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="20" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6" style="2" customWidth="1"/>
-    <col min="22" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="55" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="5.58203125" style="2"/>
     <col min="57" max="57" width="10.83203125" style="2" customWidth="1"/>
     <col min="58" max="58" width="29.25" style="2" customWidth="1"/>
@@ -21436,15 +23984,15 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
@@ -21477,10 +24025,10 @@
         <v>5</v>
       </c>
       <c r="BI6" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="BJ6" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -21508,15 +24056,15 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
-      <c r="W7" s="4"/>
+      <c r="W7" s="3"/>
       <c r="X7" s="4"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -21542,6 +24090,12 @@
       <c r="BB7" s="3"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
+      <c r="BI7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
@@ -21568,22 +24122,22 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
-      <c r="W8" s="4"/>
+      <c r="W8" s="3"/>
       <c r="X8" s="4"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="4"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="4"/>
+      <c r="AJ8" s="4"/>
+      <c r="AK8" s="4"/>
+      <c r="AL8" s="4"/>
       <c r="AM8" s="3"/>
       <c r="AN8" s="3"/>
       <c r="AO8" s="3"/>
@@ -21602,6 +24156,9 @@
       <c r="BB8" s="3"/>
       <c r="BC8" s="3"/>
       <c r="BD8" s="3"/>
+      <c r="BG8" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
@@ -21629,30 +24186,26 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="4"/>
-      <c r="X9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y9" s="3"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="3"/>
-      <c r="AP9" s="3"/>
-      <c r="AQ9" s="3"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="4"/>
+      <c r="AI9" s="4"/>
+      <c r="AJ9" s="4"/>
+      <c r="AK9" s="4"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="4"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
       <c r="AR9" s="3"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3"/>
@@ -21689,30 +24242,30 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="3"/>
+      <c r="Y10" s="4"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="3"/>
-      <c r="AQ10" s="3"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
+      <c r="AK10" s="4"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="4"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
       <c r="AT10" s="3"/>
@@ -21747,12 +24300,12 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
@@ -21760,20 +24313,20 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
       <c r="AD11" s="4"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="3"/>
-      <c r="AP11" s="3"/>
-      <c r="AQ11" s="3"/>
-      <c r="AR11" s="3"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4"/>
+      <c r="AI11" s="4"/>
+      <c r="AJ11" s="4"/>
+      <c r="AK11" s="4"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="4"/>
+      <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4"/>
       <c r="AS11" s="3"/>
       <c r="AT11" s="3"/>
       <c r="AU11" s="3"/>
@@ -21805,14 +24358,14 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
@@ -21820,25 +24373,25 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="3"/>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="3"/>
-      <c r="AR12" s="3"/>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="3"/>
-      <c r="AU12" s="3"/>
-      <c r="AV12" s="3"/>
-      <c r="AW12" s="3"/>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4"/>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="4"/>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AS12" s="4"/>
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="4"/>
+      <c r="AV12" s="4"/>
+      <c r="AW12" s="4"/>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3"/>
       <c r="AZ12" s="3"/>
@@ -21865,14 +24418,14 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
@@ -21880,9 +24433,9 @@
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AJ13" s="3"/>
@@ -21891,13 +24444,13 @@
       <c r="AM13" s="3"/>
       <c r="AN13" s="3"/>
       <c r="AO13" s="3"/>
-      <c r="AP13" s="3"/>
-      <c r="AQ13" s="3"/>
-      <c r="AR13" s="3"/>
-      <c r="AS13" s="3"/>
-      <c r="AT13" s="3"/>
-      <c r="AU13" s="3"/>
-      <c r="AV13" s="3"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="4"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3"/>
@@ -21924,25 +24477,23 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
+      <c r="Y14" s="3"/>
       <c r="Z14" s="4"/>
-      <c r="AA14" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
-      <c r="AE14" s="3"/>
+      <c r="AE14" s="4"/>
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
@@ -21954,10 +24505,10 @@
       <c r="AN14" s="3"/>
       <c r="AO14" s="3"/>
       <c r="AP14" s="3"/>
-      <c r="AQ14" s="3"/>
-      <c r="AR14" s="3"/>
-      <c r="AS14" s="3"/>
-      <c r="AT14" s="3"/>
+      <c r="AQ14" s="4"/>
+      <c r="AR14" s="4"/>
+      <c r="AS14" s="4"/>
+      <c r="AT14" s="4"/>
       <c r="AU14" s="3"/>
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
@@ -21985,20 +24536,20 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
@@ -22011,13 +24562,13 @@
       <c r="AK15" s="3"/>
       <c r="AL15" s="3"/>
       <c r="AM15" s="3"/>
-      <c r="AN15" s="3"/>
-      <c r="AO15" s="3"/>
+      <c r="AN15" s="4"/>
+      <c r="AO15" s="4"/>
       <c r="AP15" s="3"/>
-      <c r="AQ15" s="3"/>
-      <c r="AR15" s="3"/>
-      <c r="AS15" s="3"/>
-      <c r="AT15" s="3"/>
+      <c r="AQ15" s="4"/>
+      <c r="AR15" s="4"/>
+      <c r="AS15" s="4"/>
+      <c r="AT15" s="4"/>
       <c r="AU15" s="3"/>
       <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
@@ -22043,45 +24594,45 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
+      <c r="AD16" s="3"/>
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
+      <c r="AH16" s="4"/>
       <c r="AI16" s="3"/>
-      <c r="AJ16" s="3"/>
+      <c r="AJ16" s="4"/>
       <c r="AK16" s="3"/>
-      <c r="AL16" s="4"/>
-      <c r="AM16" s="4"/>
-      <c r="AN16" s="4"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="3"/>
       <c r="AO16" s="3"/>
       <c r="AP16" s="3"/>
-      <c r="AQ16" s="3"/>
-      <c r="AR16" s="3"/>
-      <c r="AS16" s="3"/>
-      <c r="AT16" s="3"/>
-      <c r="AU16" s="3"/>
-      <c r="AV16" s="3"/>
-      <c r="AW16" s="3"/>
-      <c r="AX16" s="3"/>
+      <c r="AQ16" s="4"/>
+      <c r="AR16" s="4"/>
+      <c r="AS16" s="4"/>
+      <c r="AT16" s="4"/>
+      <c r="AU16" s="4"/>
+      <c r="AV16" s="4"/>
+      <c r="AW16" s="4"/>
+      <c r="AX16" s="4"/>
       <c r="AY16" s="3"/>
       <c r="AZ16" s="3"/>
       <c r="BA16" s="3"/>
@@ -22102,15 +24653,15 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
@@ -22121,27 +24672,27 @@
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-      <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
-      <c r="AJ17" s="3"/>
-      <c r="AK17" s="3"/>
-      <c r="AL17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="3"/>
       <c r="AM17" s="3"/>
-      <c r="AN17" s="4"/>
-      <c r="AO17" s="3"/>
+      <c r="AN17" s="3"/>
+      <c r="AO17" s="4"/>
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
-      <c r="AS17" s="3"/>
-      <c r="AT17" s="3"/>
-      <c r="AU17" s="3"/>
-      <c r="AV17" s="3"/>
-      <c r="AW17" s="3"/>
-      <c r="AX17" s="3"/>
+      <c r="AS17" s="4"/>
+      <c r="AT17" s="4"/>
+      <c r="AU17" s="4"/>
+      <c r="AV17" s="4"/>
+      <c r="AW17" s="4"/>
+      <c r="AX17" s="4"/>
       <c r="AY17" s="3"/>
       <c r="AZ17" s="3"/>
       <c r="BA17" s="3"/>
@@ -22162,15 +24713,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
@@ -22181,27 +24732,27 @@
       <c r="AA18" s="4"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
       <c r="AH18" s="4"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
-      <c r="AK18" s="3"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
       <c r="AL18" s="4"/>
-      <c r="AM18" s="4"/>
-      <c r="AN18" s="4"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3"/>
       <c r="AO18" s="3"/>
       <c r="AP18" s="3"/>
-      <c r="AQ18" s="3"/>
+      <c r="AQ18" s="4"/>
       <c r="AR18" s="3"/>
-      <c r="AS18" s="3"/>
-      <c r="AT18" s="3"/>
-      <c r="AU18" s="3"/>
-      <c r="AV18" s="3"/>
-      <c r="AW18" s="3"/>
-      <c r="AX18" s="3"/>
+      <c r="AS18" s="4"/>
+      <c r="AT18" s="4"/>
+      <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="4"/>
+      <c r="AX18" s="4"/>
       <c r="AY18" s="3"/>
       <c r="AZ18" s="3"/>
       <c r="BA18" s="3"/>
@@ -22222,28 +24773,30 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
-      <c r="V19" s="3"/>
+      <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="3"/>
+      <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="3"/>
+      <c r="AB19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
-      <c r="AF19" s="3"/>
+      <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
       <c r="AH19" s="4"/>
       <c r="AI19" s="4"/>
@@ -22252,18 +24805,18 @@
       <c r="AL19" s="4"/>
       <c r="AM19" s="4"/>
       <c r="AN19" s="4"/>
-      <c r="AO19" s="3"/>
-      <c r="AP19" s="3"/>
-      <c r="AQ19" s="3"/>
-      <c r="AR19" s="3"/>
-      <c r="AS19" s="3"/>
-      <c r="AT19" s="3"/>
-      <c r="AU19" s="3"/>
-      <c r="AV19" s="3"/>
-      <c r="AW19" s="3"/>
-      <c r="AX19" s="3"/>
-      <c r="AY19" s="3"/>
-      <c r="AZ19" s="3"/>
+      <c r="AO19" s="4"/>
+      <c r="AP19" s="4"/>
+      <c r="AQ19" s="4"/>
+      <c r="AR19" s="4"/>
+      <c r="AS19" s="4"/>
+      <c r="AT19" s="4"/>
+      <c r="AU19" s="4"/>
+      <c r="AV19" s="4"/>
+      <c r="AW19" s="4"/>
+      <c r="AX19" s="4"/>
+      <c r="AY19" s="4"/>
+      <c r="AZ19" s="4"/>
       <c r="BA19" s="3"/>
       <c r="BB19" s="3"/>
       <c r="BC19" s="3"/>
@@ -22281,52 +24834,56 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
+      <c r="W20" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
+      <c r="Y20" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
-      <c r="AF20" s="4"/>
+      <c r="AF20" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4"/>
       <c r="AI20" s="4"/>
       <c r="AJ20" s="4"/>
       <c r="AK20" s="4"/>
       <c r="AL20" s="4"/>
-      <c r="AM20" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="AM20" s="4"/>
       <c r="AN20" s="4"/>
-      <c r="AO20" s="3"/>
-      <c r="AP20" s="3"/>
-      <c r="AQ20" s="3"/>
-      <c r="AR20" s="3"/>
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
-      <c r="AW20" s="3"/>
-      <c r="AX20" s="3"/>
-      <c r="AY20" s="3"/>
-      <c r="AZ20" s="3"/>
-      <c r="BA20" s="3"/>
+      <c r="AO20" s="4"/>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="4"/>
+      <c r="AR20" s="4"/>
+      <c r="AS20" s="4"/>
+      <c r="AT20" s="4"/>
+      <c r="AU20" s="4"/>
+      <c r="AV20" s="4"/>
+      <c r="AW20" s="4"/>
+      <c r="AX20" s="4"/>
+      <c r="AY20" s="4"/>
+      <c r="AZ20" s="4"/>
+      <c r="BA20" s="4"/>
       <c r="BB20" s="3"/>
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
@@ -22348,17 +24905,15 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="W21" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
@@ -22366,9 +24921,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
-      <c r="AE21" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4"/>
@@ -22378,18 +24931,18 @@
       <c r="AL21" s="4"/>
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
-      <c r="AO21" s="3"/>
-      <c r="AP21" s="3"/>
-      <c r="AQ21" s="3"/>
-      <c r="AR21" s="3"/>
-      <c r="AS21" s="3"/>
-      <c r="AT21" s="3"/>
-      <c r="AU21" s="3"/>
-      <c r="AV21" s="3"/>
-      <c r="AW21" s="3"/>
-      <c r="AX21" s="3"/>
-      <c r="AY21" s="3"/>
-      <c r="AZ21" s="3"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="4"/>
+      <c r="AQ21" s="4"/>
+      <c r="AR21" s="4"/>
+      <c r="AS21" s="4"/>
+      <c r="AT21" s="4"/>
+      <c r="AU21" s="4"/>
+      <c r="AV21" s="4"/>
+      <c r="AW21" s="4"/>
+      <c r="AX21" s="4"/>
+      <c r="AY21" s="4"/>
+      <c r="AZ21" s="4"/>
       <c r="BA21" s="3"/>
       <c r="BB21" s="3"/>
       <c r="BC21" s="3"/>
@@ -22412,44 +24965,50 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="X22" s="4"/>
-      <c r="Y22" s="3"/>
+      <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="3"/>
+      <c r="AB22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
       <c r="AE22" s="4"/>
-      <c r="AF22" s="3"/>
+      <c r="AF22" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
-      <c r="AI22" s="3"/>
-      <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
+      <c r="AI22" s="4"/>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4"/>
       <c r="AM22" s="3"/>
       <c r="AN22" s="3"/>
       <c r="AO22" s="3"/>
-      <c r="AP22" s="3"/>
-      <c r="AQ22" s="3"/>
-      <c r="AR22" s="3"/>
-      <c r="AS22" s="3"/>
-      <c r="AT22" s="3"/>
+      <c r="AP22" s="4"/>
+      <c r="AQ22" s="4"/>
+      <c r="AR22" s="4"/>
+      <c r="AS22" s="4"/>
+      <c r="AT22" s="4"/>
       <c r="AU22" s="3"/>
       <c r="AV22" s="3"/>
       <c r="AW22" s="3"/>
       <c r="AX22" s="3"/>
       <c r="AY22" s="3"/>
-      <c r="AZ22" s="3"/>
+      <c r="AZ22" s="4"/>
       <c r="BA22" s="3"/>
       <c r="BB22" s="3"/>
       <c r="BC22" s="3"/>
@@ -22472,13 +25031,13 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
+      <c r="O23" s="4"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
+      <c r="Q23" s="4"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
@@ -22492,24 +25051,26 @@
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
       <c r="AH23" s="4"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
-      <c r="AK23" s="3"/>
+      <c r="AI23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="4"/>
       <c r="AL23" s="3"/>
       <c r="AM23" s="3"/>
       <c r="AN23" s="3"/>
       <c r="AO23" s="3"/>
       <c r="AP23" s="3"/>
-      <c r="AQ23" s="3"/>
-      <c r="AR23" s="3"/>
-      <c r="AS23" s="3"/>
-      <c r="AT23" s="3"/>
+      <c r="AQ23" s="4"/>
+      <c r="AR23" s="4"/>
+      <c r="AS23" s="4"/>
+      <c r="AT23" s="4"/>
       <c r="AU23" s="3"/>
       <c r="AV23" s="3"/>
       <c r="AW23" s="3"/>
       <c r="AX23" s="3"/>
       <c r="AY23" s="3"/>
-      <c r="AZ23" s="3"/>
+      <c r="AZ23" s="4"/>
       <c r="BA23" s="3"/>
       <c r="BB23" s="3"/>
       <c r="BC23" s="3"/>
@@ -22532,45 +25093,49 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
-      <c r="AD24" s="4"/>
+      <c r="AD24" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
+      <c r="AF24" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4"/>
-      <c r="AI24" s="3"/>
-      <c r="AJ24" s="3"/>
-      <c r="AK24" s="3"/>
-      <c r="AL24" s="3"/>
-      <c r="AM24" s="3"/>
+      <c r="AI24" s="4"/>
+      <c r="AJ24" s="4"/>
+      <c r="AK24" s="4"/>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="4"/>
       <c r="AN24" s="3"/>
-      <c r="AO24" s="3"/>
-      <c r="AP24" s="3"/>
-      <c r="AQ24" s="3"/>
-      <c r="AR24" s="3"/>
-      <c r="AS24" s="3"/>
-      <c r="AT24" s="3"/>
-      <c r="AU24" s="3"/>
-      <c r="AV24" s="3"/>
-      <c r="AW24" s="3"/>
-      <c r="AX24" s="3"/>
-      <c r="AY24" s="3"/>
-      <c r="AZ24" s="3"/>
-      <c r="BA24" s="3"/>
+      <c r="AO24" s="4"/>
+      <c r="AP24" s="4"/>
+      <c r="AQ24" s="4"/>
+      <c r="AR24" s="4"/>
+      <c r="AS24" s="4"/>
+      <c r="AT24" s="4"/>
+      <c r="AU24" s="4"/>
+      <c r="AV24" s="4"/>
+      <c r="AW24" s="4"/>
+      <c r="AX24" s="4"/>
+      <c r="AY24" s="4"/>
+      <c r="AZ24" s="4"/>
+      <c r="BA24" s="4"/>
       <c r="BB24" s="3"/>
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
@@ -22601,37 +25166,47 @@
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
-      <c r="AI25" s="3"/>
-      <c r="AJ25" s="3"/>
-      <c r="AK25" s="3"/>
-      <c r="AL25" s="3"/>
-      <c r="AM25" s="3"/>
-      <c r="AN25" s="3"/>
-      <c r="AO25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH25" s="4"/>
+      <c r="AI25" s="4"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="4"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="4"/>
+      <c r="AN25" s="4"/>
+      <c r="AO25" s="4"/>
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3"/>
-      <c r="AR25" s="3"/>
-      <c r="AS25" s="3"/>
-      <c r="AT25" s="3"/>
-      <c r="AU25" s="3"/>
-      <c r="AV25" s="3"/>
+      <c r="AR25" s="4"/>
+      <c r="AS25" s="4"/>
+      <c r="AT25" s="4"/>
+      <c r="AU25" s="4"/>
+      <c r="AV25" s="4"/>
       <c r="AW25" s="3"/>
       <c r="AX25" s="3"/>
-      <c r="AY25" s="3"/>
-      <c r="AZ25" s="3"/>
-      <c r="BA25" s="3"/>
-      <c r="BB25" s="3"/>
+      <c r="AY25" s="4"/>
+      <c r="AZ25" s="4"/>
+      <c r="BA25" s="4"/>
+      <c r="BB25" s="4"/>
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
     </row>
@@ -22661,14 +25236,14 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
-      <c r="AD26" s="4"/>
-      <c r="AE26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="4"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
@@ -22681,17 +25256,17 @@
       <c r="AO26" s="3"/>
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3"/>
-      <c r="AR26" s="3"/>
-      <c r="AS26" s="3"/>
-      <c r="AT26" s="3"/>
-      <c r="AU26" s="3"/>
-      <c r="AV26" s="3"/>
+      <c r="AR26" s="4"/>
+      <c r="AS26" s="4"/>
+      <c r="AT26" s="4"/>
+      <c r="AU26" s="4"/>
+      <c r="AV26" s="4"/>
       <c r="AW26" s="3"/>
       <c r="AX26" s="3"/>
-      <c r="AY26" s="3"/>
-      <c r="AZ26" s="3"/>
-      <c r="BA26" s="3"/>
-      <c r="BB26" s="3"/>
+      <c r="AY26" s="4"/>
+      <c r="AZ26" s="4"/>
+      <c r="BA26" s="4"/>
+      <c r="BB26" s="4"/>
       <c r="BC26" s="3"/>
       <c r="BD26" s="3"/>
     </row>
@@ -22721,39 +25296,37 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
-      <c r="AD27" s="4"/>
-      <c r="AE27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="4"/>
       <c r="AF27" s="3"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
-      <c r="AJ27" s="3"/>
-      <c r="AK27" s="3"/>
-      <c r="AL27" s="3"/>
-      <c r="AM27" s="3"/>
-      <c r="AN27" s="3"/>
-      <c r="AO27" s="3"/>
-      <c r="AP27" s="3"/>
-      <c r="AQ27" s="3"/>
-      <c r="AR27" s="3"/>
-      <c r="AS27" s="3"/>
-      <c r="AT27" s="3"/>
-      <c r="AU27" s="3"/>
-      <c r="AV27" s="3"/>
-      <c r="AW27" s="3"/>
-      <c r="AX27" s="3"/>
-      <c r="AY27" s="3"/>
-      <c r="AZ27" s="3"/>
-      <c r="BA27" s="3"/>
-      <c r="BB27" s="3"/>
+      <c r="AJ27" s="4"/>
+      <c r="AK27" s="4"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="4"/>
+      <c r="AN27" s="4"/>
+      <c r="AO27" s="4"/>
+      <c r="AP27" s="4"/>
+      <c r="AQ27" s="4"/>
+      <c r="AR27" s="4"/>
+      <c r="AS27" s="4"/>
+      <c r="AT27" s="4"/>
+      <c r="AU27" s="4"/>
+      <c r="AV27" s="4"/>
+      <c r="AW27" s="4"/>
+      <c r="AX27" s="4"/>
+      <c r="AY27" s="4"/>
+      <c r="AZ27" s="4"/>
+      <c r="BA27" s="4"/>
+      <c r="BB27" s="4"/>
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
     </row>
@@ -22783,14 +25356,14 @@
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-      <c r="AC28" s="4"/>
-      <c r="AD28" s="4"/>
-      <c r="AE28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="4"/>
       <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
@@ -22799,21 +25372,21 @@
       <c r="AK28" s="3"/>
       <c r="AL28" s="3"/>
       <c r="AM28" s="3"/>
-      <c r="AN28" s="3"/>
+      <c r="AN28" s="4"/>
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
       <c r="AQ28" s="3"/>
-      <c r="AR28" s="3"/>
-      <c r="AS28" s="3"/>
+      <c r="AR28" s="4"/>
+      <c r="AS28" s="4"/>
       <c r="AT28" s="3"/>
       <c r="AU28" s="3"/>
-      <c r="AV28" s="3"/>
-      <c r="AW28" s="3"/>
-      <c r="AX28" s="3"/>
-      <c r="AY28" s="3"/>
-      <c r="AZ28" s="3"/>
-      <c r="BA28" s="3"/>
-      <c r="BB28" s="3"/>
+      <c r="AV28" s="4"/>
+      <c r="AW28" s="4"/>
+      <c r="AX28" s="4"/>
+      <c r="AY28" s="4"/>
+      <c r="AZ28" s="4"/>
+      <c r="BA28" s="4"/>
+      <c r="BB28" s="4"/>
       <c r="BC28" s="3"/>
       <c r="BD28" s="3"/>
     </row>
@@ -22834,43 +25407,43 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4"/>
-      <c r="AC29" s="4"/>
-      <c r="AD29" s="4"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
       <c r="AE29" s="4"/>
-      <c r="AF29" s="4"/>
-      <c r="AG29" s="4"/>
-      <c r="AH29" s="4"/>
-      <c r="AI29" s="4"/>
-      <c r="AJ29" s="4"/>
-      <c r="AK29" s="4"/>
-      <c r="AL29" s="4"/>
-      <c r="AM29" s="4"/>
-      <c r="AN29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="4"/>
       <c r="AO29" s="3"/>
       <c r="AP29" s="3"/>
       <c r="AQ29" s="3"/>
-      <c r="AR29" s="3"/>
-      <c r="AS29" s="3"/>
+      <c r="AR29" s="4"/>
+      <c r="AS29" s="4"/>
       <c r="AT29" s="3"/>
       <c r="AU29" s="3"/>
-      <c r="AV29" s="3"/>
-      <c r="AW29" s="3"/>
-      <c r="AX29" s="3"/>
-      <c r="AY29" s="3"/>
+      <c r="AV29" s="4"/>
+      <c r="AW29" s="4"/>
+      <c r="AX29" s="4"/>
+      <c r="AY29" s="4"/>
       <c r="AZ29" s="3"/>
       <c r="BA29" s="3"/>
       <c r="BB29" s="3"/>
@@ -22894,47 +25467,45 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z30" s="4"/>
-      <c r="AA30" s="4"/>
-      <c r="AB30" s="4"/>
-      <c r="AC30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD30" s="4"/>
-      <c r="AE30" s="4"/>
-      <c r="AF30" s="4"/>
-      <c r="AG30" s="4"/>
-      <c r="AH30" s="4"/>
-      <c r="AI30" s="4"/>
-      <c r="AJ30" s="4"/>
-      <c r="AK30" s="4"/>
-      <c r="AL30" s="4"/>
-      <c r="AM30" s="4"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
       <c r="AN30" s="3"/>
       <c r="AO30" s="3"/>
-      <c r="AP30" s="3"/>
-      <c r="AQ30" s="3"/>
-      <c r="AR30" s="3"/>
-      <c r="AS30" s="3"/>
-      <c r="AT30" s="3"/>
-      <c r="AU30" s="3"/>
-      <c r="AV30" s="3"/>
-      <c r="AW30" s="3"/>
-      <c r="AX30" s="3"/>
-      <c r="AY30" s="3"/>
+      <c r="AP30" s="4"/>
+      <c r="AQ30" s="4"/>
+      <c r="AR30" s="4"/>
+      <c r="AS30" s="4"/>
+      <c r="AT30" s="4"/>
+      <c r="AU30" s="4"/>
+      <c r="AV30" s="4"/>
+      <c r="AW30" s="4"/>
+      <c r="AX30" s="4"/>
+      <c r="AY30" s="4"/>
       <c r="AZ30" s="3"/>
       <c r="BA30" s="3"/>
       <c r="BB30" s="3"/>
@@ -22958,35 +25529,33 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
-      <c r="AA31" s="4"/>
-      <c r="AB31" s="4"/>
-      <c r="AC31" s="4"/>
-      <c r="AD31" s="4"/>
-      <c r="AE31" s="4"/>
-      <c r="AF31" s="4"/>
-      <c r="AG31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH31" s="4"/>
-      <c r="AI31" s="4"/>
-      <c r="AJ31" s="4"/>
-      <c r="AK31" s="4"/>
-      <c r="AL31" s="4"/>
-      <c r="AM31" s="4"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
       <c r="AO31" s="3"/>
       <c r="AP31" s="3"/>
@@ -22994,10 +25563,10 @@
       <c r="AR31" s="3"/>
       <c r="AS31" s="3"/>
       <c r="AT31" s="3"/>
-      <c r="AU31" s="3"/>
-      <c r="AV31" s="3"/>
-      <c r="AW31" s="3"/>
-      <c r="AX31" s="3"/>
+      <c r="AU31" s="4"/>
+      <c r="AV31" s="4"/>
+      <c r="AW31" s="4"/>
+      <c r="AX31" s="4"/>
       <c r="AY31" s="3"/>
       <c r="AZ31" s="3"/>
       <c r="BA31" s="3"/>
@@ -23022,31 +25591,33 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-      <c r="AD32" s="4"/>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
-      <c r="AG32" s="4"/>
-      <c r="AH32" s="4"/>
-      <c r="AI32" s="4"/>
-      <c r="AJ32" s="4"/>
-      <c r="AK32" s="4"/>
-      <c r="AL32" s="4"/>
-      <c r="AM32" s="4"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
       <c r="AN32" s="3"/>
       <c r="AO32" s="3"/>
       <c r="AP32" s="3"/>
@@ -23082,31 +25653,33 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
-      <c r="AD33" s="4"/>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
-      <c r="AG33" s="4"/>
-      <c r="AH33" s="4"/>
-      <c r="AI33" s="4"/>
-      <c r="AJ33" s="4"/>
-      <c r="AK33" s="4"/>
-      <c r="AL33" s="4"/>
-      <c r="AM33" s="4"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
       <c r="AN33" s="3"/>
       <c r="AO33" s="3"/>
       <c r="AP33" s="3"/>
@@ -23142,33 +25715,33 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA34" s="4"/>
-      <c r="AB34" s="4"/>
-      <c r="AC34" s="4"/>
-      <c r="AD34" s="4"/>
-      <c r="AE34" s="4"/>
-      <c r="AF34" s="4"/>
-      <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="4"/>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="4"/>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="4"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
       <c r="AN34" s="3"/>
       <c r="AO34" s="3"/>
       <c r="AP34" s="3"/>
@@ -23204,31 +25777,31 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
-      <c r="AC35" s="4"/>
-      <c r="AD35" s="4"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
       <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="4"/>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="4"/>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="4"/>
+      <c r="AF35" s="3"/>
+      <c r="AG35" s="3"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="3"/>
+      <c r="AJ35" s="3"/>
+      <c r="AK35" s="3"/>
+      <c r="AL35" s="3"/>
+      <c r="AM35" s="3"/>
       <c r="AN35" s="3"/>
       <c r="AO35" s="3"/>
       <c r="AP35" s="3"/>
@@ -23273,14 +25846,14 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
-      <c r="AA36" s="4"/>
-      <c r="AB36" s="4"/>
-      <c r="AC36" s="4"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="3"/>
+      <c r="AE36" s="4"/>
       <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
@@ -23333,16 +25906,16 @@
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
+      <c r="AE37" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="AF37" s="3"/>
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
@@ -23432,7 +26005,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -23441,8 +26014,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="20" zoomScaleNormal="20" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="BF25" sqref="BF25"/>
+    <sheetView tabSelected="1" topLeftCell="M13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.58203125" defaultRowHeight="35.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -24058,6 +26631,12 @@
       <c r="BB7" s="3"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
+      <c r="BI7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:62" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
@@ -24209,9 +26788,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="Y10" s="9"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="3"/>
@@ -24223,9 +26800,7 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
-      <c r="AK10" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="AK10" s="9"/>
       <c r="AL10" s="4"/>
       <c r="AM10" s="4"/>
       <c r="AN10" s="4"/>
@@ -24397,11 +26972,21 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
-      <c r="AG13" s="4"/>
+      <c r="AC13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="AH13" s="4"/>
       <c r="AI13" s="4"/>
       <c r="AJ13" s="4"/>
@@ -24451,27 +27036,33 @@
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-      <c r="W14" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="W14" s="9"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
-      <c r="AG14" s="4"/>
+      <c r="AC14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG14" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="AH14" s="4"/>
       <c r="AI14" s="4"/>
       <c r="AJ14" s="3"/>
       <c r="AK14" s="3"/>
       <c r="AL14" s="4"/>
-      <c r="AM14" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
@@ -24522,9 +27113,11 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
+      <c r="AD15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
       <c r="AH15" s="4"/>
       <c r="AI15" s="4"/>
@@ -24582,9 +27175,9 @@
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
       <c r="AH16" s="4"/>
       <c r="AI16" s="4"/>
@@ -24640,13 +27233,17 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
+      <c r="AB17" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="AC17" s="4"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
-      <c r="AH17" s="4"/>
+      <c r="AH17" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
       <c r="AK17" s="4"/>
@@ -24759,9 +27356,15 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="4"/>
+      <c r="AA19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC19" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
@@ -24819,15 +27422,25 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
+      <c r="AA20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
-      <c r="AH20" s="4"/>
-      <c r="AI20" s="4"/>
+      <c r="AH20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI20" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
       <c r="AL20" s="4"/>
@@ -24875,9 +27488,7 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="W21" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="W21" s="9"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
@@ -24888,14 +27499,16 @@
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
+      <c r="AH21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI21" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="AJ21" s="3"/>
       <c r="AK21" s="3"/>
       <c r="AL21" s="4"/>
-      <c r="AM21" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="AM21" s="9"/>
       <c r="AN21" s="4"/>
       <c r="AO21" s="4"/>
       <c r="AP21" s="4"/>
@@ -24947,7 +27560,9 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
-      <c r="AE22" s="4"/>
+      <c r="AE22" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
@@ -25177,9 +27792,7 @@
       <c r="R26" s="3"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="U26" s="9"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
@@ -25199,9 +27812,7 @@
       <c r="AL26" s="3"/>
       <c r="AM26" s="4"/>
       <c r="AN26" s="4"/>
-      <c r="AO26" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="AO26" s="9"/>
       <c r="AP26" s="4"/>
       <c r="AQ26" s="4"/>
       <c r="AR26" s="3"/>
@@ -25671,9 +28282,7 @@
       <c r="AB34" s="4"/>
       <c r="AC34" s="4"/>
       <c r="AD34" s="4"/>
-      <c r="AE34" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="AE34" s="9"/>
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
       <c r="AH34" s="4"/>
@@ -25952,7 +28561,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:BJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="30" zoomScaleNormal="30" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="N14" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="AG22" sqref="AG22"/>
     </sheetView>
   </sheetViews>

</xml_diff>